<commit_message>
trabajando en multiregistro ajax
</commit_message>
<xml_diff>
--- a/directory/formats/Formato_Multiregistro.xlsx
+++ b/directory/formats/Formato_Multiregistro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\tutorias\directory\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FEA9D8B-37B2-45C1-8D82-B8B02D1C554A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91FE15D-6AE6-4FCC-9C77-D3B4061E69D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nombre</t>
   </si>
@@ -34,19 +34,16 @@
     <t>Sexo</t>
   </si>
   <si>
-    <t>NumeroControl</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
-    <t>Carrera/Especialidad</t>
+    <t>Ncontrol/Matricula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -430,11 +427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G65"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -442,11 +439,10 @@
     <col min="1" max="3" width="50.7109375" style="2" customWidth="1"/>
     <col min="4" max="4" width="17.7109375" style="2" customWidth="1"/>
     <col min="5" max="5" width="34.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="50.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.15" customHeight="1">
+    <row r="1" spans="1:6" ht="28.15" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,134 +456,116 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2"/>
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
       <c r="E2"/>
-      <c r="F2"/>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3"/>
       <c r="B3"/>
       <c r="C3"/>
       <c r="D3"/>
       <c r="E3"/>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:7">
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4"/>
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4"/>
       <c r="E4"/>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9"/>
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:7">
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:7">
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
       <c r="D12"/>
       <c r="E12"/>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:7">
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:7">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:7">
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:7">
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
-      <c r="F16"/>
     </row>
     <row r="17" customFormat="1"/>
     <row r="18" customFormat="1"/>

</xml_diff>